<commit_message>
Add Export and Hierarchy Components
</commit_message>
<xml_diff>
--- a/server/employee_data_export.xlsx
+++ b/server/employee_data_export.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="31">
   <si>
     <t>firstName</t>
   </si>
@@ -143,8 +143,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -157,7 +169,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -433,6 +445,476 @@
         <v>17</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D10" t="n" s="0">
+        <v>100.0</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F10" t="n" s="7">
+        <v>45257.0</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="H10" t="n" s="0">
+        <v>1001.0</v>
+      </c>
+      <c r="I10" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="J10" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="K10" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0"/>
+      <c r="B11" s="0"/>
+      <c r="C11" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D11" s="0"/>
+      <c r="E11" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F11" s="0"/>
+      <c r="G11" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="H11" s="0"/>
+      <c r="I11" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="J11" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="K11" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D12" t="n" s="0">
+        <v>767.0</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F12" t="n" s="8">
+        <v>45257.229166666664</v>
+      </c>
+      <c r="G12" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="H12" t="n" s="0">
+        <v>3688.0</v>
+      </c>
+      <c r="I12" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="J12" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="K12" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D13" t="n" s="0">
+        <v>767.0</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F13" t="n" s="9">
+        <v>45257.229166666664</v>
+      </c>
+      <c r="G13" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="H13" t="n" s="0">
+        <v>3688.0</v>
+      </c>
+      <c r="I13" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="J13" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="K13" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D14" t="n" s="0">
+        <v>767.0</v>
+      </c>
+      <c r="E14" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F14" t="n" s="10">
+        <v>45257.229166666664</v>
+      </c>
+      <c r="G14" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="H14" t="n" s="0">
+        <v>3688.0</v>
+      </c>
+      <c r="I14" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="J14" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="K14" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D15" t="n" s="0">
+        <v>767.0</v>
+      </c>
+      <c r="E15" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F15" t="n" s="11">
+        <v>45257.229166666664</v>
+      </c>
+      <c r="G15" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="H15" t="n" s="0">
+        <v>3688.0</v>
+      </c>
+      <c r="I15" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="J15" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="K15" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D16" t="n" s="0">
+        <v>767.0</v>
+      </c>
+      <c r="E16" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F16" t="n" s="12">
+        <v>45257.229166666664</v>
+      </c>
+      <c r="G16" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="H16" t="n" s="0">
+        <v>3688.0</v>
+      </c>
+      <c r="I16" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="J16" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="K16" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D17" t="n" s="0">
+        <v>100.0</v>
+      </c>
+      <c r="E17" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F17" t="n" s="13">
+        <v>45257.0</v>
+      </c>
+      <c r="G17" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="H17" t="n" s="0">
+        <v>1001.0</v>
+      </c>
+      <c r="I17" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="J17" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="K17" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0"/>
+      <c r="B18" s="0"/>
+      <c r="C18" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D18" s="0"/>
+      <c r="E18" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F18" s="0"/>
+      <c r="G18" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="H18" s="0"/>
+      <c r="I18" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="J18" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="K18" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D19" t="n" s="0">
+        <v>767.0</v>
+      </c>
+      <c r="E19" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F19" t="n" s="14">
+        <v>45257.229166666664</v>
+      </c>
+      <c r="G19" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="H19" t="n" s="0">
+        <v>3688.0</v>
+      </c>
+      <c r="I19" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="J19" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="K19" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D20" t="n" s="0">
+        <v>767.0</v>
+      </c>
+      <c r="E20" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F20" t="n" s="15">
+        <v>45257.229166666664</v>
+      </c>
+      <c r="G20" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="H20" t="n" s="0">
+        <v>3688.0</v>
+      </c>
+      <c r="I20" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="J20" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="K20" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D21" t="n" s="0">
+        <v>767.0</v>
+      </c>
+      <c r="E21" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F21" t="n" s="16">
+        <v>45257.229166666664</v>
+      </c>
+      <c r="G21" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="H21" t="n" s="0">
+        <v>3688.0</v>
+      </c>
+      <c r="I21" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="J21" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="K21" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D22" t="n" s="0">
+        <v>767.0</v>
+      </c>
+      <c r="E22" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F22" t="n" s="17">
+        <v>45257.229166666664</v>
+      </c>
+      <c r="G22" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="H22" t="n" s="0">
+        <v>3688.0</v>
+      </c>
+      <c r="I22" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="J22" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="K22" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D23" t="n" s="0">
+        <v>767.0</v>
+      </c>
+      <c r="E23" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F23" t="n" s="18">
+        <v>45257.229166666664</v>
+      </c>
+      <c r="G23" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="H23" t="n" s="0">
+        <v>3688.0</v>
+      </c>
+      <c r="I23" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="J23" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="K23" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Add view team and view hierarchy feature
</commit_message>
<xml_diff>
--- a/server/employee_data_export.xlsx
+++ b/server/employee_data_export.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="54">
   <si>
     <t>firstName</t>
   </si>
@@ -236,7 +236,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -300,7 +300,7 @@
         <v>15</v>
       </c>
       <c r="H3" t="n" s="0">
-        <v>3456.0</v>
+        <v>3.0</v>
       </c>
       <c r="I3" t="n" s="0">
         <v>2.0</v>
@@ -370,7 +370,7 @@
         <v>15</v>
       </c>
       <c r="H5" t="n" s="0">
-        <v>70283.0</v>
+        <v>3.0</v>
       </c>
       <c r="I5" t="n" s="0">
         <v>4.0</v>
@@ -440,7 +440,7 @@
         <v>15</v>
       </c>
       <c r="H7" t="n" s="0">
-        <v>3688.0</v>
+        <v>3.0</v>
       </c>
       <c r="I7" t="n" s="0">
         <v>6.0</v>
@@ -475,7 +475,7 @@
         <v>15</v>
       </c>
       <c r="H8" t="n" s="0">
-        <v>3688.0</v>
+        <v>3.0</v>
       </c>
       <c r="I8" t="n" s="0">
         <v>7.0</v>
@@ -863,6 +863,35 @@
         <v>53</v>
       </c>
       <c r="K19" t="s" s="0">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D20" s="0"/>
+      <c r="E20" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="F20" s="0"/>
+      <c r="G20" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="H20" s="0"/>
+      <c r="I20" t="n" s="0">
+        <v>19.0</v>
+      </c>
+      <c r="J20" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="K20" t="s" s="0">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update styling and key-result page
</commit_message>
<xml_diff>
--- a/server/employee_data_export.xlsx
+++ b/server/employee_data_export.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="54">
   <si>
     <t>firstName</t>
   </si>
@@ -236,7 +236,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -405,7 +405,7 @@
         <v>15</v>
       </c>
       <c r="H6" t="n" s="0">
-        <v>725.0</v>
+        <v>2.0</v>
       </c>
       <c r="I6" t="n" s="0">
         <v>5.0</v>
@@ -510,7 +510,7 @@
         <v>15</v>
       </c>
       <c r="H9" t="n" s="0">
-        <v>3688.0</v>
+        <v>2.0</v>
       </c>
       <c r="I9" t="n" s="0">
         <v>8.0</v>
@@ -545,7 +545,7 @@
         <v>15</v>
       </c>
       <c r="H10" t="n" s="0">
-        <v>3688.0</v>
+        <v>5.0</v>
       </c>
       <c r="I10" t="n" s="0">
         <v>9.0</v>
@@ -580,7 +580,7 @@
         <v>15</v>
       </c>
       <c r="H11" t="n" s="0">
-        <v>3688.0</v>
+        <v>5.0</v>
       </c>
       <c r="I11" t="n" s="0">
         <v>10.0</v>
@@ -615,7 +615,7 @@
         <v>51</v>
       </c>
       <c r="H12" t="n" s="0">
-        <v>3612.0</v>
+        <v>8.0</v>
       </c>
       <c r="I12" t="n" s="0">
         <v>11.0</v>
@@ -650,7 +650,7 @@
         <v>15</v>
       </c>
       <c r="H13" t="n" s="0">
-        <v>3688.0</v>
+        <v>8.0</v>
       </c>
       <c r="I13" t="n" s="0">
         <v>12.0</v>
@@ -894,6 +894,54 @@
       <c r="K20" t="s" s="0">
         <v>53</v>
       </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D21" s="0"/>
+      <c r="E21" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="F21" s="0"/>
+      <c r="G21" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="H21" s="0"/>
+      <c r="I21" t="n" s="0">
+        <v>20.0</v>
+      </c>
+      <c r="J21" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="K21" t="s" s="0">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0"/>
+      <c r="B22" s="0"/>
+      <c r="C22" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D22" s="0"/>
+      <c r="E22" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="F22" s="0"/>
+      <c r="G22" s="0"/>
+      <c r="H22" s="0"/>
+      <c r="I22" t="n" s="0">
+        <v>21.0</v>
+      </c>
+      <c r="J22" s="0"/>
+      <c r="K22" s="0"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>